<commit_message>
added traceability matrix (moscow) document
</commit_message>
<xml_diff>
--- a/Documentation/SoftwareDevImplementPlan.xlsx
+++ b/Documentation/SoftwareDevImplementPlan.xlsx
@@ -1,11 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23223"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87201FF5-FE0E-42CC-B8A9-89406EE443B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20026893\Documents\styleme\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Task_Table" sheetId="1" r:id="rId1"/>
@@ -16,7 +20,7 @@
     <definedName name="Resource_Table">Resource_Table!$A$1:$L$1</definedName>
     <definedName name="Task_Table">Task_Table!$A$1:$I$1</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -150,21 +154,12 @@
     <t>Performance metrics</t>
   </si>
   <si>
-    <t>Move code to production environment (AWS)</t>
-  </si>
-  <si>
     <t>Deployment Phase</t>
   </si>
   <si>
-    <t>Test live environment</t>
-  </si>
-  <si>
     <t>Implement logging</t>
   </si>
   <si>
-    <t>Performance metrics (live)</t>
-  </si>
-  <si>
     <t>Validate requirements with clients</t>
   </si>
   <si>
@@ -271,17 +266,23 @@
   </si>
   <si>
     <t>Deployment Team</t>
+  </si>
+  <si>
+    <t>Move code to cloud environment (AWS)</t>
+  </si>
+  <si>
+    <t>Present prototype to clients</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,23 +479,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -530,23 +514,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -722,14 +689,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="76.7109375" style="1" customWidth="1"/>
@@ -742,7 +709,7 @@
     <col min="9" max="9" width="114.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -767,7 +734,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>7</v>
       </c>
@@ -782,7 +749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>ROW() - 2</f>
         <v>1</v>
@@ -794,7 +761,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D71" si="0">_xlfn.DAYS(F3, E3)</f>
+        <f t="shared" ref="D3:D33" si="0">_xlfn.DAYS(F3, E3)</f>
         <v>18</v>
       </c>
       <c r="E3" s="3">
@@ -804,7 +771,7 @@
         <v>44078</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A10" si="1">ROW() - 2</f>
         <v>2</v>
@@ -826,7 +793,7 @@
         <v>44078</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -848,7 +815,7 @@
         <v>44078</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -870,7 +837,7 @@
         <v>44078</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -894,7 +861,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -916,7 +883,7 @@
         <v>44081</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -938,7 +905,7 @@
         <v>44078</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -963,7 +930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="18.75">
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>19</v>
       </c>
@@ -977,7 +944,7 @@
       <c r="I11" s="13"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>ROW() - 3</f>
         <v>9</v>
@@ -999,77 +966,73 @@
         <v>44081</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="1">
-        <v>10</v>
-      </c>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="2">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E13" s="3">
         <v>44081</v>
       </c>
       <c r="F13" s="3">
-        <v>44088</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f t="shared" ref="A14:A79" si="2">ROW() - 3</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E14" s="3">
         <v>44081</v>
       </c>
       <c r="F14" s="3">
+        <v>44088</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f t="shared" ref="A15:A78" si="2">ROW() - 3</f>
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E15" s="3">
+        <v>44081</v>
+      </c>
+      <c r="F15" s="3">
         <v>44086</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="1">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E15" s="3">
-        <v>44088</v>
-      </c>
-      <c r="F15" s="3">
-        <v>44093</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>10</v>
@@ -1085,104 +1048,104 @@
         <v>44093</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E17" s="3">
+        <v>44088</v>
+      </c>
+      <c r="F17" s="3">
+        <v>44093</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E18" s="3">
         <v>44095</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F18" s="3">
         <v>44102</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="1">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E19" s="3">
         <v>44067</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F19" s="3">
         <v>44072</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="1">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E20" s="3">
         <v>44096</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F20" s="3">
         <v>44109</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E20" s="3">
-        <v>44109</v>
-      </c>
-      <c r="F20" s="3">
-        <v>44117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
@@ -1195,103 +1158,103 @@
         <v>44117</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E22" s="3">
         <v>44109</v>
       </c>
       <c r="F22" s="3">
+        <v>44117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E23" s="3">
+        <v>44109</v>
+      </c>
+      <c r="F23" s="3">
         <v>44114</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="1">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="2">
+      <c r="C24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
-      </c>
-      <c r="E23" s="3">
-        <v>44116</v>
-      </c>
-      <c r="F23" s="3">
-        <v>44130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="1">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
       </c>
       <c r="E24" s="3">
         <v>44116</v>
       </c>
       <c r="F24" s="3">
+        <v>44130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E25" s="3">
+        <v>44116</v>
+      </c>
+      <c r="F25" s="3">
         <v>44121</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="1">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="B25" s="1" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E25" s="3">
-        <v>44109</v>
-      </c>
-      <c r="F25" s="3">
-        <v>44117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="1">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="2">
@@ -1305,113 +1268,113 @@
         <v>44117</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="2">
+        <f>_xlfn.DAYS(F27, E27)</f>
+        <v>14</v>
+      </c>
+      <c r="E27" s="3">
+        <v>44128</v>
+      </c>
+      <c r="F27" s="3">
+        <v>44142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E28" s="3">
+        <v>44109</v>
+      </c>
+      <c r="F28" s="3">
+        <v>44117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="C29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E29" s="3">
         <v>44117</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F29" s="3">
         <v>44121</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="1">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="B28" s="1" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="2">
+      <c r="C30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E30" s="3">
         <v>44123</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F30" s="3">
         <v>44128</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="1">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="B29" s="1" t="s">
+    <row r="31" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="E29" s="3">
-        <v>44128</v>
-      </c>
-      <c r="F29" s="3">
-        <v>44142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="18.75">
-      <c r="A30" s="16" t="s">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="1">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="E31" s="3">
-        <v>44113</v>
-      </c>
-      <c r="F31" s="3">
-        <v>44120</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="1">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>31</v>
@@ -1427,13 +1390,13 @@
         <v>44129</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>10</v>
@@ -1443,35 +1406,22 @@
         <v>7</v>
       </c>
       <c r="E33" s="3">
-        <v>44114</v>
+        <v>44121</v>
       </c>
       <c r="F33" s="3">
-        <v>44121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>44128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="E34" s="3">
-        <v>44121</v>
-      </c>
-      <c r="F34" s="3">
-        <v>44128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="D34" s="2"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -1480,7 +1430,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -1489,7 +1439,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -1498,7 +1448,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -1507,7 +1457,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -1516,7 +1466,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -1525,7 +1475,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -1534,7 +1484,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -1543,7 +1493,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -1552,7 +1502,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -1561,7 +1511,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -1570,7 +1520,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -1579,7 +1529,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -1588,7 +1538,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -1597,7 +1547,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -1606,7 +1556,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -1615,7 +1565,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -1624,7 +1574,7 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -1633,7 +1583,7 @@
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -1642,7 +1592,7 @@
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -1651,7 +1601,7 @@
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f t="shared" si="2"/>
         <v>52</v>
@@ -1660,7 +1610,7 @@
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f t="shared" si="2"/>
         <v>53</v>
@@ -1669,7 +1619,7 @@
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f t="shared" si="2"/>
         <v>54</v>
@@ -1678,7 +1628,7 @@
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -1687,7 +1637,7 @@
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f t="shared" si="2"/>
         <v>56</v>
@@ -1696,7 +1646,7 @@
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -1705,7 +1655,7 @@
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f t="shared" si="2"/>
         <v>58</v>
@@ -1714,7 +1664,7 @@
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -1723,7 +1673,7 @@
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f t="shared" si="2"/>
         <v>60</v>
@@ -1732,7 +1682,7 @@
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f t="shared" si="2"/>
         <v>61</v>
@@ -1741,7 +1691,7 @@
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="2"/>
         <v>62</v>
@@ -1750,7 +1700,7 @@
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="2"/>
         <v>63</v>
@@ -1759,7 +1709,7 @@
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="2"/>
         <v>64</v>
@@ -1768,7 +1718,7 @@
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f t="shared" si="2"/>
         <v>65</v>
@@ -1777,7 +1727,7 @@
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f t="shared" si="2"/>
         <v>66</v>
@@ -1786,7 +1736,7 @@
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f t="shared" si="2"/>
         <v>67</v>
@@ -1795,7 +1745,7 @@
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" si="2"/>
         <v>68</v>
@@ -1804,7 +1754,7 @@
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="2"/>
         <v>69</v>
@@ -1813,7 +1763,7 @@
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="2"/>
         <v>70</v>
@@ -1822,7 +1772,7 @@
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f t="shared" si="2"/>
         <v>71</v>
@@ -1831,7 +1781,7 @@
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f t="shared" si="2"/>
         <v>72</v>
@@ -1840,7 +1790,7 @@
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f t="shared" si="2"/>
         <v>73</v>
@@ -1849,7 +1799,7 @@
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f t="shared" si="2"/>
         <v>74</v>
@@ -1858,7 +1808,7 @@
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" si="2"/>
         <v>75</v>
@@ -1867,25 +1817,25 @@
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A79:A92" si="3">ROW() - 3</f>
         <v>76</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <f t="shared" ref="A80:A93" si="3">ROW() - 3</f>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f t="shared" si="3"/>
         <v>78</v>
@@ -1894,7 +1844,7 @@
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f t="shared" si="3"/>
         <v>79</v>
@@ -1903,7 +1853,7 @@
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f t="shared" si="3"/>
         <v>80</v>
@@ -1912,7 +1862,7 @@
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f t="shared" si="3"/>
         <v>81</v>
@@ -1921,7 +1871,7 @@
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f t="shared" si="3"/>
         <v>82</v>
@@ -1930,7 +1880,7 @@
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f t="shared" si="3"/>
         <v>83</v>
@@ -1939,7 +1889,7 @@
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <f t="shared" si="3"/>
         <v>84</v>
@@ -1948,7 +1898,7 @@
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <f t="shared" si="3"/>
         <v>85</v>
@@ -1957,7 +1907,7 @@
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <f t="shared" si="3"/>
         <v>86</v>
@@ -1966,7 +1916,7 @@
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <f t="shared" si="3"/>
         <v>87</v>
@@ -1975,7 +1925,7 @@
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <f t="shared" si="3"/>
         <v>88</v>
@@ -1984,7 +1934,7 @@
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <f t="shared" si="3"/>
         <v>89</v>
@@ -1992,278 +1942,269 @@
       <c r="D92" s="2"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
-    </row>
-    <row r="93" spans="1:6">
-      <c r="A93" s="1">
-        <f t="shared" si="3"/>
-        <v>90</v>
-      </c>
-      <c r="D93" s="2"/>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A31:H31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView topLeftCell="C5" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="37.42578125" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>51</v>
-      </c>
-      <c r="I1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" t="s">
-        <v>54</v>
       </c>
       <c r="L1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" t="s">
         <v>55</v>
       </c>
-      <c r="D2" t="s">
+      <c r="K2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>56</v>
       </c>
-      <c r="I2" t="s">
+      <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="J2" t="s">
+      <c r="C3" t="s">
         <v>58</v>
       </c>
-      <c r="K2" t="s">
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>59</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>60</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>61</v>
       </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>62</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>64</v>
       </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>65</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>67</v>
       </c>
-      <c r="D5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
+      <c r="K6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>68</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>69</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>70</v>
       </c>
-      <c r="D6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s">
+      <c r="K7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>71</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>72</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>73</v>
       </c>
-      <c r="D7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" t="s">
-        <v>57</v>
-      </c>
-      <c r="J7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="K9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>75</v>
       </c>
-      <c r="C8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" t="s">
-        <v>57</v>
-      </c>
-      <c r="J8" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" t="s">
-        <v>58</v>
-      </c>
-      <c r="K9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" t="s">
-        <v>58</v>
-      </c>
       <c r="K10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added app website to implementation plan
</commit_message>
<xml_diff>
--- a/Documentation/SoftwareDevImplementPlan.xlsx
+++ b/Documentation/SoftwareDevImplementPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23229"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB3ACBA3-DA29-40EB-99A3-5535860E5DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="459" documentId="11_A630CA59DDA3301160A6DC93A8264671BB1A27BF" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{957FEA34-882C-4A65-90CB-7939ACB0379B}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Performance metrics (live)</t>
+  </si>
+  <si>
+    <t>Deploy simple static website for the app</t>
   </si>
   <si>
     <t>Deliver the project</t>
@@ -315,9 +318,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -343,6 +343,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -726,16 +729,16 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
       <c r="I2" s="14" t="s">
         <v>8</v>
       </c>
@@ -752,7 +755,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D39" si="0">_xlfn.DAYS(F3, E3)</f>
+        <f t="shared" ref="D3:D40" si="0">_xlfn.DAYS(F3, E3)</f>
         <v>18</v>
       </c>
       <c r="E3" s="3">
@@ -917,21 +920,21 @@
       <c r="F10" s="3">
         <v>44174</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="I10" s="27" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="18.75">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
       <c r="I11" s="13"/>
       <c r="J11" s="7"/>
     </row>
@@ -1352,44 +1355,44 @@
         <v>44137</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="20" customFormat="1" ht="15.75">
-      <c r="A31" s="16">
+    <row r="31" spans="1:9" s="19" customFormat="1" ht="15.75">
+      <c r="A31" s="15">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="17">
+      <c r="C31" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="16">
         <f>_xlfn.DAYS(F31, E31)</f>
         <v>7</v>
       </c>
-      <c r="E31" s="18">
+      <c r="E31" s="17">
         <v>44137</v>
       </c>
-      <c r="F31" s="18">
+      <c r="F31" s="17">
         <v>44144</v>
       </c>
-      <c r="G31" s="19"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="21" t="s">
+      <c r="G31" s="18"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="20" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="18.75">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1">
@@ -1415,7 +1418,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1">
-        <f t="shared" ref="A34:A39" si="3">ROW() - 4</f>
+        <f t="shared" ref="A34:A40" si="3">ROW() - 4</f>
         <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1523,45 +1526,58 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="26" customFormat="1" ht="15.75">
-      <c r="A39" s="22">
+    <row r="39" spans="1:9">
+      <c r="A39" s="1">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="23">
+      <c r="C39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E39" s="3">
+        <v>44153</v>
+      </c>
+      <c r="F39" s="3">
+        <v>44155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="25" customFormat="1" ht="15.75">
+      <c r="A40" s="21">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E40" s="23">
         <v>44156</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F40" s="23">
         <v>44156</v>
       </c>
-      <c r="G39" s="25"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="1">
-        <f t="shared" ref="A39:A83" si="4">ROW() - 3</f>
-        <v>37</v>
-      </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="26" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="A40:A84" si="4">ROW() - 3</f>
         <v>38</v>
       </c>
       <c r="D41" s="2"/>
@@ -1948,7 +1964,7 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="1">
-        <f t="shared" ref="A84:A97" si="5">ROW() - 3</f>
+        <f t="shared" si="4"/>
         <v>81</v>
       </c>
       <c r="D84" s="2"/>
@@ -1957,7 +1973,7 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="A85:A98" si="5">ROW() - 3</f>
         <v>82</v>
       </c>
       <c r="D85" s="2"/>
@@ -2071,6 +2087,15 @@
       <c r="D97" s="2"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="1">
+        <f t="shared" si="5"/>
+        <v>95</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>